<commit_message>
"Actualizado con capturas y confi.toml"
</commit_message>
<xml_diff>
--- a/predictions/Orense_Future_Predictions.xlsx
+++ b/predictions/Orense_Future_Predictions.xlsx
@@ -438,7 +438,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K12"/>
+  <dimension ref="A1:K9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -830,123 +830,6 @@
         </is>
       </c>
     </row>
-    <row r="10">
-      <c r="A10" s="2" t="inlineStr">
-        <is>
-          <t>08/01/2025</t>
-        </is>
-      </c>
-      <c r="B10" s="2" t="n">
-        <v>12.152</v>
-      </c>
-      <c r="C10" s="2" t="n">
-        <v>8.133000000000004</v>
-      </c>
-      <c r="D10" s="2" t="n">
-        <v>16.361</v>
-      </c>
-      <c r="E10" s="2" t="n">
-        <v>4.444999999999999</v>
-      </c>
-      <c r="F10" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="G10" s="2" t="n">
-        <v>192.06</v>
-      </c>
-      <c r="H10" s="2" t="n">
-        <v>13.469</v>
-      </c>
-      <c r="I10" s="2" t="n">
-        <v>30</v>
-      </c>
-      <c r="J10" s="2" t="n">
-        <v>1017.992</v>
-      </c>
-      <c r="K10" s="2" t="inlineStr">
-        <is>
-          <t>Orense</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" s="2" t="inlineStr">
-        <is>
-          <t>09/01/2025</t>
-        </is>
-      </c>
-      <c r="B11" s="2" t="n">
-        <v>12.223</v>
-      </c>
-      <c r="C11" s="2" t="n">
-        <v>9.505000000000003</v>
-      </c>
-      <c r="D11" s="2" t="n">
-        <v>17.298</v>
-      </c>
-      <c r="E11" s="2" t="n">
-        <v>4.029999999999998</v>
-      </c>
-      <c r="F11" s="2" t="n">
-        <v>0.1</v>
-      </c>
-      <c r="G11" s="2" t="n">
-        <v>195.15</v>
-      </c>
-      <c r="H11" s="2" t="n">
-        <v>12.291</v>
-      </c>
-      <c r="I11" s="2" t="n">
-        <v>30</v>
-      </c>
-      <c r="J11" s="2" t="n">
-        <v>1016.422</v>
-      </c>
-      <c r="K11" s="2" t="inlineStr">
-        <is>
-          <t>Orense</t>
-        </is>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" s="2" t="inlineStr">
-        <is>
-          <t>10/01/2025</t>
-        </is>
-      </c>
-      <c r="B12" s="2" t="n">
-        <v>12.609</v>
-      </c>
-      <c r="C12" s="2" t="n">
-        <v>9.043000000000005</v>
-      </c>
-      <c r="D12" s="2" t="n">
-        <v>17.182</v>
-      </c>
-      <c r="E12" s="2" t="n">
-        <v>3.238999999999999</v>
-      </c>
-      <c r="F12" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="G12" s="2" t="n">
-        <v>208.84</v>
-      </c>
-      <c r="H12" s="2" t="n">
-        <v>11.258</v>
-      </c>
-      <c r="I12" s="2" t="n">
-        <v>30</v>
-      </c>
-      <c r="J12" s="2" t="n">
-        <v>1015.127</v>
-      </c>
-      <c r="K12" s="2" t="inlineStr">
-        <is>
-          <t>Orense</t>
-        </is>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>